<commit_message>
status update for hybris dev
</commit_message>
<xml_diff>
--- a/docs/bio metric integration estimation/Face recognition Dev Plan_v1.xlsx
+++ b/docs/bio metric integration estimation/Face recognition Dev Plan_v1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="65">
   <si>
     <t>Functionality</t>
   </si>
@@ -99,45 +99,9 @@
     <t>13. Add method persistNewUser to existing controller MDIYImageQualityCheckController</t>
   </si>
   <si>
-    <t>8. Create MDIYSaveBiometricDataFacade</t>
-  </si>
-  <si>
-    <t>9. Create MDIYSaveBiometricDataFacadeImpl</t>
-  </si>
-  <si>
-    <t>11. Create cronjob MDIYPersistUserCronJob</t>
-  </si>
-  <si>
-    <t>13. Create Controller MDIYSubmitUserController</t>
-  </si>
-  <si>
     <t>d. Modify dependencies on classes inside qrcodeaddon</t>
   </si>
   <si>
-    <t>8. Create MDIYSubmitUserFacade</t>
-  </si>
-  <si>
-    <t>9. Create MDIYSubmitUserFacadeImpl</t>
-  </si>
-  <si>
-    <t>10. Create MDIYSubmitUserService</t>
-  </si>
-  <si>
-    <t>11. Create MDYSubmitUserServiceImpl</t>
-  </si>
-  <si>
-    <t>10. Create MDIYSubmitUserDao</t>
-  </si>
-  <si>
-    <t>11. Create MDYSubmitUserDaoImpl</t>
-  </si>
-  <si>
-    <t>12. Create MDIYCSRCustomerPopulator</t>
-  </si>
-  <si>
-    <t>13. Create MDIYImagePopulator</t>
-  </si>
-  <si>
     <t xml:space="preserve">               a. Declare variables and methods</t>
   </si>
   <si>
@@ -195,16 +159,58 @@
     <t>Completed</t>
   </si>
   <si>
-    <t>In progress</t>
-  </si>
-  <si>
     <t>Swarnima</t>
   </si>
   <si>
     <t>Swapnil</t>
   </si>
   <si>
-    <t>dependent</t>
+    <t>In progress(dependent)</t>
+  </si>
+  <si>
+    <t>14. Create MDIYSaveBiometricDataFacade</t>
+  </si>
+  <si>
+    <t>15. Create MDIYSaveBiometricDataFacadeImpl</t>
+  </si>
+  <si>
+    <t>16. Create MDIYCustomerDataService</t>
+  </si>
+  <si>
+    <t>17. Create MDIYSaveCustomerDataServiceImpl</t>
+  </si>
+  <si>
+    <t>18. Create cronjob MDIYPersistUserCronJob</t>
+  </si>
+  <si>
+    <t>19. Create Controller MDIYSubmitUserController</t>
+  </si>
+  <si>
+    <t>20. Create MDIYSubmitUserFacade</t>
+  </si>
+  <si>
+    <t>21. Create MDIYSubmitUserFacadeImpl</t>
+  </si>
+  <si>
+    <t>22. Create MDIYSubmitUserService</t>
+  </si>
+  <si>
+    <t>23. Create MDYSubmitUserServiceImpl</t>
+  </si>
+  <si>
+    <t>24. Create MDIYSubmitUserDao</t>
+  </si>
+  <si>
+    <t>25. Create MDYSubmitUserDaoImpl</t>
+  </si>
+  <si>
+    <t>26. Create MDIYCSRCustomerPopulator</t>
+  </si>
+  <si>
+    <t>27. Create MDIYImagePopulator</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -651,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J56"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,16 +697,16 @@
         <v>5</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -716,84 +722,72 @@
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3">
-        <v>2</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="3">
-        <v>2</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" s="9">
-        <v>42212</v>
-      </c>
-      <c r="I3" s="9">
-        <v>42212</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3">
-        <v>19</v>
-      </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="9">
+        <v>42212</v>
+      </c>
+      <c r="I4" s="9">
+        <v>42212</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="3">
-        <v>3</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H5" s="9">
-        <v>42212</v>
-      </c>
-      <c r="I5" s="9">
-        <v>42212</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="F5" s="3">
+        <v>19</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="H6" s="9">
         <v>42212</v>
@@ -802,104 +796,102 @@
         <v>42212</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="3">
-        <v>4</v>
-      </c>
-      <c r="C7" s="11">
-        <v>2</v>
-      </c>
-      <c r="D7" s="11">
-        <v>2</v>
-      </c>
-      <c r="E7" s="11">
-        <v>4</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="H7" s="9">
-        <v>42213</v>
+        <v>42212</v>
       </c>
       <c r="I7" s="9">
-        <v>42214</v>
+        <v>42212</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B8" s="3">
-        <v>2</v>
-      </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
+        <v>4</v>
+      </c>
+      <c r="C8" s="11">
+        <v>2</v>
+      </c>
+      <c r="D8" s="11">
+        <v>2</v>
+      </c>
+      <c r="E8" s="11">
+        <v>4</v>
+      </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="H8" s="9">
         <v>42213</v>
       </c>
       <c r="I8" s="9">
-        <v>42214</v>
+        <v>42216</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="A9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="3">
-        <v>4</v>
-      </c>
+      <c r="G9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="9">
+        <v>42213</v>
+      </c>
+      <c r="I9" s="9">
+        <v>42216</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="3">
-        <v>4</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" s="9">
-        <v>42209</v>
-      </c>
-      <c r="I10" s="9">
-        <v>42209</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B11" s="3">
         <v>4</v>
@@ -911,7 +903,7 @@
         <v>4</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="H11" s="9">
         <v>42209</v>
@@ -920,50 +912,50 @@
         <v>42209</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="H12" s="9">
-        <v>42212</v>
+        <v>42209</v>
       </c>
       <c r="I12" s="9">
-        <v>42212</v>
+        <v>42209</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="H13" s="9">
         <v>42212</v>
@@ -972,68 +964,70 @@
         <v>42212</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="B14" s="3">
+        <v>4</v>
+      </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3">
-        <v>16</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="9">
+        <v>42212</v>
+      </c>
+      <c r="I14" s="9">
+        <v>42212</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3">
+        <v>16</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B16" s="3">
         <v>4</v>
       </c>
-      <c r="C15" s="11">
-        <v>2</v>
-      </c>
-      <c r="D15" s="11">
-        <v>2</v>
-      </c>
-      <c r="E15" s="11">
-        <v>2</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H15" s="9">
-        <v>42212</v>
-      </c>
-      <c r="I15" s="9">
-        <v>42212</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="3">
-        <v>2</v>
-      </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
+      <c r="C16" s="11">
+        <v>2</v>
+      </c>
+      <c r="D16" s="11">
+        <v>2</v>
+      </c>
+      <c r="E16" s="11">
+        <v>2</v>
+      </c>
       <c r="F16" s="3"/>
-      <c r="G16" s="10" t="s">
-        <v>61</v>
+      <c r="G16" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="H16" s="9">
         <v>42212</v>
@@ -1042,203 +1036,223 @@
         <v>42212</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" s="3">
-        <v>4</v>
-      </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
+        <v>2</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
       <c r="F17" s="3"/>
       <c r="G17" s="10" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="H17" s="9">
         <v>42212</v>
       </c>
       <c r="I17" s="9">
-        <v>42214</v>
+        <v>42212</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B18" s="3">
-        <v>1</v>
-      </c>
-      <c r="C18" s="11">
-        <v>2</v>
-      </c>
-      <c r="D18" s="11">
-        <v>2</v>
-      </c>
-      <c r="E18" s="11">
         <v>4</v>
       </c>
-      <c r="F18" s="3">
-        <v>22</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>57</v>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="H18" s="9">
-        <v>42213</v>
+        <v>42212</v>
       </c>
       <c r="I18" s="9">
-        <v>42213</v>
+        <v>42216</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+      <c r="C19" s="11">
+        <v>2</v>
+      </c>
+      <c r="D19" s="11">
+        <v>2</v>
+      </c>
+      <c r="E19" s="11">
+        <v>4</v>
+      </c>
+      <c r="F19" s="3">
         <v>22</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="3"/>
-      <c r="I19" s="3"/>
+      <c r="G19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="9">
+        <v>42213</v>
+      </c>
+      <c r="I19" s="9">
+        <v>42213</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="3">
-        <v>4</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B20" s="3"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H20" s="9">
-        <v>42213</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B21" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="H21" s="9">
         <v>42213</v>
       </c>
-      <c r="I21" s="3" t="s">
-        <v>62</v>
+      <c r="I21" s="9">
+        <v>42216</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="B22" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
+      <c r="G22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H22" s="9">
+        <v>42213</v>
+      </c>
+      <c r="I22" s="9">
+        <v>42216</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
       <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
+      <c r="G23" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H23" s="9">
+        <v>42215</v>
+      </c>
+      <c r="I23" s="9">
+        <v>42215</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="3">
+        <v>24</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="3">
         <v>6</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-    </row>
-    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H25" s="9">
+        <v>42215</v>
+      </c>
+      <c r="I25" s="9">
+        <v>42215</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="8">
-        <v>2</v>
-      </c>
-      <c r="D25" s="8">
-        <v>2</v>
-      </c>
-      <c r="E25" s="8">
-        <v>2</v>
-      </c>
-      <c r="F25" s="3">
+      <c r="B26" s="3"/>
+      <c r="C26" s="8">
+        <v>2</v>
+      </c>
+      <c r="D26" s="8">
+        <v>2</v>
+      </c>
+      <c r="E26" s="8">
+        <v>2</v>
+      </c>
+      <c r="F26" s="3">
         <v>12</v>
       </c>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="3">
-        <v>4</v>
-      </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
@@ -1246,23 +1260,31 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B27" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
+      <c r="G27" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H27" s="9">
+        <v>42215</v>
+      </c>
+      <c r="I27" s="9">
+        <v>42216</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B28" s="3">
         <v>2</v>
@@ -1271,136 +1293,186 @@
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-    </row>
-    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="G28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" s="9">
+        <v>42215</v>
+      </c>
+      <c r="I28" s="9">
+        <v>42216</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B29" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
-      <c r="F29" s="3">
+      <c r="F29" s="3"/>
+      <c r="G29" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H29" s="9">
+        <v>42215</v>
+      </c>
+      <c r="I29" s="9">
+        <v>42216</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="3">
+        <v>4</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="11">
         <v>17</v>
       </c>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B30" s="3">
-        <v>1</v>
-      </c>
-      <c r="C30" s="11">
-        <v>2</v>
-      </c>
-      <c r="D30" s="11">
-        <v>2</v>
-      </c>
-      <c r="E30" s="11">
-        <v>2</v>
-      </c>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
+      <c r="G30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H30" s="9">
+        <v>42219</v>
+      </c>
+      <c r="I30" s="9">
+        <v>42219</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="11">
+        <v>2</v>
+      </c>
+      <c r="D31" s="11">
+        <v>2</v>
+      </c>
+      <c r="E31" s="11">
+        <v>2</v>
+      </c>
+      <c r="F31" s="12"/>
+      <c r="G31" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H31" s="9">
+        <v>42219</v>
+      </c>
+      <c r="I31" s="9">
+        <v>42219</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
-      <c r="F32" s="3"/>
+      <c r="F32" s="12"/>
       <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
       <c r="J32" s="3"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B33" s="3">
+        <v>28</v>
+      </c>
+      <c r="B33" s="11">
         <v>2</v>
       </c>
       <c r="C33" s="12"/>
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H33" s="9">
+        <v>42219</v>
+      </c>
+      <c r="I33" s="9">
+        <v>42219</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="3">
-        <v>1</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B34" s="13"/>
       <c r="C34" s="12"/>
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H34" s="9">
+        <v>42220</v>
+      </c>
+      <c r="I34" s="9">
+        <v>42220</v>
+      </c>
       <c r="J34" s="3"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="3"/>
+        <v>52</v>
+      </c>
+      <c r="B35" s="3">
+        <v>1</v>
+      </c>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H35" s="9">
+        <v>42220</v>
+      </c>
+      <c r="I35" s="9">
+        <v>42220</v>
+      </c>
       <c r="J35" s="3"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B36" s="3">
-        <v>3</v>
-      </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
+        <v>53</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="13"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
@@ -1408,55 +1480,61 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B37" s="3">
+        <v>3</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H37" s="9">
+        <v>42220</v>
+      </c>
+      <c r="I37" s="9">
+        <v>42220</v>
+      </c>
+      <c r="J37" s="3"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="3">
         <v>6</v>
       </c>
-      <c r="C37" s="8">
-        <v>2</v>
-      </c>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8">
-        <v>2</v>
-      </c>
-      <c r="F37" s="3">
+      <c r="C38" s="8">
+        <v>2</v>
+      </c>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8">
+        <v>2</v>
+      </c>
+      <c r="F38" s="3">
         <v>10</v>
       </c>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
+      <c r="G38" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H38" s="9">
+        <v>42221</v>
+      </c>
+      <c r="I38" s="9">
+        <v>42223</v>
+      </c>
       <c r="J38" s="3"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="A39" s="2"/>
       <c r="B39" s="3"/>
-      <c r="C39" s="11">
-        <v>2</v>
-      </c>
-      <c r="D39" s="11">
-        <v>2</v>
-      </c>
-      <c r="E39" s="11">
-        <v>4</v>
-      </c>
-      <c r="F39" s="3">
-        <v>31</v>
-      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
@@ -1464,39 +1542,53 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B40" s="3">
-        <v>3</v>
-      </c>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="3"/>
+        <v>55</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="11">
+        <v>2</v>
+      </c>
+      <c r="D40" s="11">
+        <v>2</v>
+      </c>
+      <c r="E40" s="11">
+        <v>4</v>
+      </c>
+      <c r="F40" s="3">
+        <v>31</v>
+      </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="3"/>
+      <c r="A41" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" s="3">
+        <v>3</v>
+      </c>
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
       <c r="E41" s="12"/>
       <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
+      <c r="G41" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H41" s="9">
+        <v>42219</v>
+      </c>
+      <c r="I41" s="9">
+        <v>42219</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B42" s="3">
-        <v>1</v>
-      </c>
+      <c r="A42" s="2"/>
+      <c r="B42" s="3"/>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
@@ -1508,25 +1600,33 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B43" s="3"/>
+        <v>56</v>
+      </c>
+      <c r="B43" s="3">
+        <v>1</v>
+      </c>
       <c r="C43" s="12"/>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
       <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
+      <c r="G43" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H43" s="9">
+        <v>42219</v>
+      </c>
+      <c r="I43" s="9">
+        <v>42219</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B44" s="3">
-        <v>4</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="B44" s="3"/>
       <c r="C44" s="12"/>
       <c r="D44" s="12"/>
       <c r="E44" s="12"/>
@@ -1538,41 +1638,55 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B45" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C45" s="12"/>
       <c r="D45" s="12"/>
       <c r="E45" s="12"/>
       <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
+      <c r="G45" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H45" s="9">
+        <v>42219</v>
+      </c>
+      <c r="I45" s="9">
+        <v>42219</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B46" s="3"/>
+        <v>58</v>
+      </c>
+      <c r="B46" s="3">
+        <v>1</v>
+      </c>
       <c r="C46" s="12"/>
       <c r="D46" s="12"/>
       <c r="E46" s="12"/>
       <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
+      <c r="G46" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H46" s="9">
+        <v>42220</v>
+      </c>
+      <c r="I46" s="9">
+        <v>42220</v>
+      </c>
       <c r="J46" s="3"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B47" s="3">
-        <v>3</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="B47" s="3"/>
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
       <c r="E47" s="12"/>
@@ -1584,41 +1698,53 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B48" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
       <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
+      <c r="G48" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H48" s="9">
+        <v>42220</v>
+      </c>
+      <c r="I48" s="9">
+        <v>42220</v>
+      </c>
       <c r="J48" s="3"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B49" s="3"/>
+        <v>60</v>
+      </c>
+      <c r="B49" s="3">
+        <v>1</v>
+      </c>
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
       <c r="E49" s="12"/>
       <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
+      <c r="G49" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H49" s="9">
+        <v>42220</v>
+      </c>
+      <c r="I49" s="9">
+        <v>42220</v>
+      </c>
       <c r="J49" s="3"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B50" s="3">
-        <v>3</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B50" s="3"/>
       <c r="C50" s="12"/>
       <c r="D50" s="12"/>
       <c r="E50" s="12"/>
@@ -1630,7 +1756,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B51" s="3">
         <v>3</v>
@@ -1639,100 +1765,136 @@
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
       <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
+      <c r="G51" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H51" s="9">
+        <v>42220</v>
+      </c>
+      <c r="I51" s="9">
+        <v>42220</v>
+      </c>
       <c r="J51" s="3"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="B52" s="3">
+        <v>3</v>
+      </c>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H52" s="9">
+        <v>42221</v>
+      </c>
+      <c r="I52" s="9">
+        <v>42221</v>
+      </c>
+      <c r="J52" s="3"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B53" s="3">
         <v>4</v>
       </c>
-      <c r="C52" s="13"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
       <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
+      <c r="G53" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H53" s="9">
+        <v>42221</v>
+      </c>
+      <c r="I53" s="9">
+        <v>42222</v>
+      </c>
       <c r="J53" s="3"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
-      <c r="F54" s="3">
-        <v>9</v>
-      </c>
+      <c r="F54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
+      <c r="A55" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
+      <c r="F55" s="3">
+        <v>9</v>
+      </c>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
-        <v>7</v>
-      </c>
+      <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
-      <c r="F56" s="7">
-        <v>150</v>
-      </c>
+      <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
     </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="7">
+        <v>150</v>
+      </c>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="3"/>
+      <c r="J57" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="D18:D23"/>
-    <mergeCell ref="E18:E23"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="C39:C52"/>
-    <mergeCell ref="D39:D52"/>
-    <mergeCell ref="E39:E52"/>
-    <mergeCell ref="C30:C35"/>
-    <mergeCell ref="D30:D35"/>
-    <mergeCell ref="E30:E35"/>
+  <mergeCells count="17">
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C40:C53"/>
+    <mergeCell ref="D40:D53"/>
+    <mergeCell ref="E40:E53"/>
+    <mergeCell ref="D19:D24"/>
+    <mergeCell ref="E19:E24"/>
+    <mergeCell ref="F30:F36"/>
+    <mergeCell ref="C31:C36"/>
+    <mergeCell ref="D31:D36"/>
+    <mergeCell ref="E31:E36"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="C19:C24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated tasks and status for Hybris
</commit_message>
<xml_diff>
--- a/docs/bio metric integration estimation/Face recognition Dev Plan_v1.xlsx
+++ b/docs/bio metric integration estimation/Face recognition Dev Plan_v1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="67">
   <si>
     <t>Functionality</t>
   </si>
@@ -36,9 +36,6 @@
     <t>TOTAL(hours)</t>
   </si>
   <si>
-    <t>Configuration</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -211,6 +208,15 @@
   </si>
   <si>
     <t>In Progress</t>
+  </si>
+  <si>
+    <t>28. Configuration</t>
+  </si>
+  <si>
+    <t>29. Create webservice controller for sending image threshold configuration value to IOS(MDIYConfigurationController)</t>
+  </si>
+  <si>
+    <t>30. Create a webservice controller for sending all images uploaded by a customer to IOS(MDIYCustomerImagesController)</t>
   </si>
 </sst>
 </file>
@@ -347,10 +353,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -657,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J57"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,16 +703,16 @@
         <v>5</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -735,7 +741,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3">
         <v>2</v>
@@ -747,7 +753,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H4" s="9">
         <v>42212</v>
@@ -756,12 +762,12 @@
         <v>42212</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -777,7 +783,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3">
         <v>3</v>
@@ -787,7 +793,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H6" s="9">
         <v>42212</v>
@@ -796,12 +802,12 @@
         <v>42212</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="3">
         <v>2</v>
@@ -811,7 +817,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H7" s="9">
         <v>42212</v>
@@ -820,12 +826,12 @@
         <v>42212</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
@@ -841,7 +847,7 @@
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H8" s="9">
         <v>42213</v>
@@ -850,22 +856,22 @@
         <v>42216</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="3">
         <v>2</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H9" s="9">
         <v>42213</v>
@@ -874,7 +880,7 @@
         <v>42216</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -891,7 +897,7 @@
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="3">
         <v>4</v>
@@ -903,7 +909,7 @@
         <v>4</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H11" s="9">
         <v>42209</v>
@@ -912,12 +918,12 @@
         <v>42209</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="3">
         <v>4</v>
@@ -929,7 +935,7 @@
         <v>4</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H12" s="9">
         <v>42209</v>
@@ -938,12 +944,12 @@
         <v>42209</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="3">
         <v>2</v>
@@ -955,7 +961,7 @@
         <v>2</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H13" s="9">
         <v>42212</v>
@@ -964,12 +970,12 @@
         <v>42212</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="3">
         <v>4</v>
@@ -981,7 +987,7 @@
         <v>4</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H14" s="9">
         <v>42212</v>
@@ -990,12 +996,12 @@
         <v>42212</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1011,7 +1017,7 @@
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="3">
         <v>4</v>
@@ -1027,7 +1033,7 @@
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H16" s="9">
         <v>42212</v>
@@ -1036,22 +1042,22 @@
         <v>42212</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="3">
         <v>2</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
       <c r="F17" s="3"/>
       <c r="G17" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H17" s="9">
         <v>42212</v>
@@ -1060,22 +1066,22 @@
         <v>42212</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="3">
         <v>4</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
       <c r="F18" s="3"/>
       <c r="G18" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H18" s="9">
         <v>42212</v>
@@ -1084,12 +1090,12 @@
         <v>42216</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="3">
         <v>1</v>
@@ -1107,7 +1113,7 @@
         <v>22</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H19" s="9">
         <v>42213</v>
@@ -1116,33 +1122,33 @@
         <v>42213</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="3"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
       <c r="F20" s="3"/>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" s="3">
         <v>4</v>
       </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H21" s="9">
         <v>42213</v>
@@ -1151,22 +1157,22 @@
         <v>42216</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" s="3">
         <v>2</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H22" s="9">
         <v>42213</v>
@@ -1175,22 +1181,22 @@
         <v>42216</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="3">
         <v>1</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H23" s="9">
         <v>42215</v>
@@ -1199,22 +1205,22 @@
         <v>42215</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
       <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="3">
         <v>6</v>
@@ -1224,7 +1230,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H25" s="9">
         <v>42215</v>
@@ -1233,12 +1239,12 @@
         <v>42215</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="8">
@@ -1251,7 +1257,7 @@
         <v>2</v>
       </c>
       <c r="F26" s="3">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -1260,7 +1266,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27" s="3">
         <v>4</v>
@@ -1270,7 +1276,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H27" s="9">
         <v>42215</v>
@@ -1279,12 +1285,12 @@
         <v>42216</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28" s="3">
         <v>2</v>
@@ -1294,7 +1300,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H28" s="9">
         <v>42215</v>
@@ -1303,12 +1309,12 @@
         <v>42216</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="3">
         <v>2</v>
@@ -1318,7 +1324,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H29" s="9">
         <v>42215</v>
@@ -1327,12 +1333,12 @@
         <v>42216</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" s="3">
         <v>4</v>
@@ -1344,7 +1350,7 @@
         <v>17</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H30" s="9">
         <v>42219</v>
@@ -1353,12 +1359,12 @@
         <v>42219</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B31" s="3">
         <v>1</v>
@@ -1372,9 +1378,9 @@
       <c r="E31" s="11">
         <v>2</v>
       </c>
-      <c r="F31" s="12"/>
+      <c r="F31" s="13"/>
       <c r="G31" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H31" s="9">
         <v>42219</v>
@@ -1383,34 +1389,34 @@
         <v>42219</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B32" s="3"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
       <c r="G32" s="3"/>
       <c r="J32" s="3"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B33" s="11">
         <v>2</v>
       </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
       <c r="G33" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H33" s="9">
         <v>42219</v>
@@ -1419,20 +1425,20 @@
         <v>42219</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
+        <v>29</v>
+      </c>
+      <c r="B34" s="12"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
       <c r="G34" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H34" s="9">
         <v>42220</v>
@@ -1440,21 +1446,23 @@
       <c r="I34" s="9">
         <v>42220</v>
       </c>
-      <c r="J34" s="3"/>
+      <c r="J34" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B35" s="3">
         <v>1</v>
       </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
       <c r="G35" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H35" s="9">
         <v>42220</v>
@@ -1462,17 +1470,19 @@
       <c r="I35" s="9">
         <v>42220</v>
       </c>
-      <c r="J35" s="3"/>
+      <c r="J35" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B36" s="3"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="12"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
@@ -1480,7 +1490,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B37" s="3">
         <v>3</v>
@@ -1490,7 +1500,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H37" s="9">
         <v>42220</v>
@@ -1498,11 +1508,13 @@
       <c r="I37" s="9">
         <v>42220</v>
       </c>
-      <c r="J37" s="3"/>
+      <c r="J37" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B38" s="3">
         <v>6</v>
@@ -1518,7 +1530,7 @@
         <v>10</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H38" s="9">
         <v>42221</v>
@@ -1542,7 +1554,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="11">
@@ -1564,17 +1576,17 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B41" s="3">
         <v>3</v>
       </c>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H41" s="9">
         <v>42219</v>
@@ -1583,15 +1595,15 @@
         <v>42219</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="3"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
@@ -1600,17 +1612,17 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B43" s="3">
         <v>1</v>
       </c>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H43" s="9">
         <v>42219</v>
@@ -1619,17 +1631,17 @@
         <v>42219</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B44" s="3"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
@@ -1638,17 +1650,17 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B45" s="3">
         <v>4</v>
       </c>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H45" s="9">
         <v>42219</v>
@@ -1657,22 +1669,22 @@
         <v>42219</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B46" s="3">
         <v>1</v>
       </c>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H46" s="9">
         <v>42220</v>
@@ -1680,16 +1692,18 @@
       <c r="I46" s="9">
         <v>42220</v>
       </c>
-      <c r="J46" s="3"/>
+      <c r="J46" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B47" s="3"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
@@ -1698,17 +1712,17 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B48" s="3">
         <v>3</v>
       </c>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H48" s="9">
         <v>42220</v>
@@ -1716,38 +1730,40 @@
       <c r="I48" s="9">
         <v>42220</v>
       </c>
-      <c r="J48" s="3"/>
+      <c r="J48" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B49" s="3">
         <v>1</v>
       </c>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H49" s="9">
-        <v>42220</v>
+        <v>42221</v>
       </c>
       <c r="I49" s="9">
-        <v>42220</v>
+        <v>42221</v>
       </c>
       <c r="J49" s="3"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B50" s="3"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
@@ -1756,67 +1772,67 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B51" s="3">
         <v>3</v>
       </c>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H51" s="9">
-        <v>42220</v>
+        <v>42221</v>
       </c>
       <c r="I51" s="9">
-        <v>42220</v>
+        <v>42222</v>
       </c>
       <c r="J51" s="3"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B52" s="3">
         <v>3</v>
       </c>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H52" s="9">
         <v>42221</v>
       </c>
       <c r="I52" s="9">
-        <v>42221</v>
+        <v>42222</v>
       </c>
       <c r="J52" s="3"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B53" s="3">
         <v>4</v>
       </c>
-      <c r="C53" s="13"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="13"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H53" s="9">
         <v>42221</v>
       </c>
       <c r="I53" s="9">
-        <v>42222</v>
+        <v>42223</v>
       </c>
       <c r="J53" s="3"/>
     </row>
@@ -1834,7 +1850,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -1848,42 +1864,74 @@
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
+    <row r="56" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56" s="3">
+        <v>3</v>
+      </c>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
-      <c r="J56" s="3"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B57" s="3"/>
+      <c r="F56" s="3">
+        <v>3</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H56" s="9">
+        <v>42220</v>
+      </c>
+      <c r="I56" s="9">
+        <v>42220</v>
+      </c>
+      <c r="J56" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" s="3">
+        <v>5</v>
+      </c>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
-      <c r="F57" s="7">
-        <v>150</v>
-      </c>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
+      <c r="F57" s="3">
+        <v>5</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H57" s="9">
+        <v>42221</v>
+      </c>
+      <c r="I57" s="9">
+        <v>42221</v>
+      </c>
       <c r="J57" s="3"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="7">
+        <v>158</v>
+      </c>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C40:C53"/>
-    <mergeCell ref="D40:D53"/>
-    <mergeCell ref="E40:E53"/>
-    <mergeCell ref="D19:D24"/>
-    <mergeCell ref="E19:E24"/>
     <mergeCell ref="F30:F36"/>
     <mergeCell ref="C31:C36"/>
     <mergeCell ref="D31:D36"/>
@@ -1895,6 +1943,12 @@
     <mergeCell ref="D16:D18"/>
     <mergeCell ref="E16:E18"/>
     <mergeCell ref="C19:C24"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C40:C53"/>
+    <mergeCell ref="D40:D53"/>
+    <mergeCell ref="E40:E53"/>
+    <mergeCell ref="D19:D24"/>
+    <mergeCell ref="E19:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated tasks and assignee
</commit_message>
<xml_diff>
--- a/docs/bio metric integration estimation/Face recognition Dev Plan_v1.xlsx
+++ b/docs/bio metric integration estimation/Face recognition Dev Plan_v1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="71">
   <si>
     <t>Functionality</t>
   </si>
@@ -63,9 +63,6 @@
     <t>a. Create controller with  GET method(MDIYImageQualityCheckController)</t>
   </si>
   <si>
-    <t>c. Create the method saveCustomerDetails which is triggered on load of profile pic</t>
-  </si>
-  <si>
     <t>4. Add itemtypes</t>
   </si>
   <si>
@@ -220,6 +217,18 @@
   </si>
   <si>
     <t>Completed(dependent)</t>
+  </si>
+  <si>
+    <t>In Progress(Modification)</t>
+  </si>
+  <si>
+    <t>31. UI Integration with new files</t>
+  </si>
+  <si>
+    <t>a. Integrate separate files for CSR dashboard</t>
+  </si>
+  <si>
+    <t>b. Integrate separate files for Orders dashboard</t>
   </si>
 </sst>
 </file>
@@ -329,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -361,6 +370,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -666,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J58"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="J56" sqref="J56"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="N59" sqref="N59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,16 +725,16 @@
         <v>5</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -756,7 +775,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H4" s="9">
         <v>42212</v>
@@ -765,7 +784,7 @@
         <v>42212</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -796,7 +815,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H6" s="9">
         <v>42212</v>
@@ -805,7 +824,7 @@
         <v>42212</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -820,7 +839,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H7" s="9">
         <v>42212</v>
@@ -829,7 +848,7 @@
         <v>42212</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -850,7 +869,7 @@
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H8" s="9">
         <v>42213</v>
@@ -859,12 +878,12 @@
         <v>42216</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="3">
         <v>2</v>
@@ -874,7 +893,7 @@
       <c r="E9" s="12"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H9" s="9">
         <v>42213</v>
@@ -883,7 +902,7 @@
         <v>42216</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -912,7 +931,7 @@
         <v>4</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H11" s="9">
         <v>42209</v>
@@ -921,12 +940,12 @@
         <v>42209</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="3">
         <v>4</v>
@@ -938,7 +957,7 @@
         <v>4</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H12" s="9">
         <v>42209</v>
@@ -947,12 +966,12 @@
         <v>42209</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="3">
         <v>2</v>
@@ -964,7 +983,7 @@
         <v>2</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H13" s="9">
         <v>42212</v>
@@ -973,12 +992,12 @@
         <v>42212</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="3">
         <v>4</v>
@@ -990,7 +1009,7 @@
         <v>4</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H14" s="9">
         <v>42212</v>
@@ -999,19 +1018,19 @@
         <v>42212</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -1035,8 +1054,8 @@
         <v>2</v>
       </c>
       <c r="F16" s="3"/>
-      <c r="G16" s="3" t="s">
-        <v>44</v>
+      <c r="G16" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="H16" s="9">
         <v>42212</v>
@@ -1045,7 +1064,7 @@
         <v>42212</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1060,7 +1079,7 @@
       <c r="E17" s="13"/>
       <c r="F17" s="3"/>
       <c r="G17" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H17" s="9">
         <v>42212</v>
@@ -1069,36 +1088,24 @@
         <v>42212</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="3">
-        <v>4</v>
-      </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="H18" s="9">
-        <v>42212</v>
-      </c>
-      <c r="I18" s="9">
-        <v>42216</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="G18" s="10"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="3"/>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="3">
         <v>1</v>
@@ -1115,22 +1122,22 @@
       <c r="F19" s="3">
         <v>22</v>
       </c>
-      <c r="G19" s="3" t="s">
-        <v>44</v>
+      <c r="G19" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="H19" s="9">
-        <v>42213</v>
+        <v>42223</v>
       </c>
       <c r="I19" s="9">
-        <v>42213</v>
+        <v>42223</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="13"/>
@@ -1141,7 +1148,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" s="3">
         <v>4</v>
@@ -1150,22 +1157,22 @@
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="3" t="s">
-        <v>44</v>
+      <c r="G21" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="H21" s="9">
-        <v>42213</v>
+        <v>42223</v>
       </c>
       <c r="I21" s="9">
-        <v>42216</v>
+        <v>42223</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22" s="3">
         <v>2</v>
@@ -1174,22 +1181,22 @@
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="3" t="s">
-        <v>44</v>
+      <c r="G22" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="H22" s="9">
-        <v>42213</v>
+        <v>42226</v>
       </c>
       <c r="I22" s="9">
-        <v>42216</v>
+        <v>42226</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="3">
         <v>1</v>
@@ -1198,22 +1205,22 @@
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
       <c r="F23" s="3"/>
-      <c r="G23" s="3" t="s">
-        <v>44</v>
+      <c r="G23" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="H23" s="9">
-        <v>42215</v>
+        <v>42226</v>
       </c>
       <c r="I23" s="9">
-        <v>42215</v>
+        <v>42226</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="13"/>
@@ -1223,7 +1230,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" s="3">
         <v>6</v>
@@ -1232,22 +1239,22 @@
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="3" t="s">
-        <v>44</v>
+      <c r="G25" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="H25" s="9">
-        <v>42215</v>
+        <v>42226</v>
       </c>
       <c r="I25" s="9">
-        <v>42215</v>
+        <v>42227</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="8">
@@ -1269,7 +1276,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="3">
         <v>4</v>
@@ -1279,21 +1286,21 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H27" s="9">
-        <v>42215</v>
+        <v>42227</v>
       </c>
       <c r="I27" s="9">
-        <v>42216</v>
+        <v>42227</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="3">
         <v>2</v>
@@ -1303,21 +1310,21 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H28" s="9">
-        <v>42215</v>
+        <v>42227</v>
       </c>
       <c r="I28" s="9">
-        <v>42216</v>
+        <v>42227</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29" s="3">
         <v>2</v>
@@ -1327,21 +1334,21 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H29" s="9">
-        <v>42215</v>
+        <v>42227</v>
       </c>
       <c r="I29" s="9">
-        <v>42216</v>
+        <v>42227</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B30" s="3">
         <v>4</v>
@@ -1349,25 +1356,25 @@
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="11">
+      <c r="F30" s="15">
         <v>17</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>44</v>
+      <c r="G30" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="H30" s="9">
-        <v>42219</v>
+        <v>42228</v>
       </c>
       <c r="I30" s="9">
-        <v>42219</v>
+        <v>42228</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B31" s="3">
         <v>1</v>
@@ -1381,35 +1388,35 @@
       <c r="E31" s="11">
         <v>2</v>
       </c>
-      <c r="F31" s="13"/>
-      <c r="G31" s="3" t="s">
-        <v>44</v>
+      <c r="F31" s="16"/>
+      <c r="G31" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="H31" s="9">
-        <v>42219</v>
+        <v>42228</v>
       </c>
       <c r="I31" s="9">
-        <v>42219</v>
+        <v>42228</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
       <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
+      <c r="F32" s="16"/>
       <c r="G32" s="3"/>
       <c r="J32" s="3"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B33" s="11">
         <v>2</v>
@@ -1417,45 +1424,45 @@
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
       <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="3" t="s">
-        <v>44</v>
+      <c r="F33" s="16"/>
+      <c r="G33" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="H33" s="9">
-        <v>42219</v>
+        <v>42229</v>
       </c>
       <c r="I33" s="9">
-        <v>42219</v>
+        <v>42229</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B34" s="12"/>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
       <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="3" t="s">
-        <v>44</v>
+      <c r="F34" s="16"/>
+      <c r="G34" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="H34" s="9">
-        <v>42220</v>
+        <v>42229</v>
       </c>
       <c r="I34" s="9">
-        <v>42220</v>
+        <v>42229</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B35" s="3">
         <v>1</v>
@@ -1463,29 +1470,29 @@
       <c r="C35" s="13"/>
       <c r="D35" s="13"/>
       <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="3" t="s">
-        <v>44</v>
+      <c r="F35" s="16"/>
+      <c r="G35" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="H35" s="9">
-        <v>42220</v>
+        <v>42229</v>
       </c>
       <c r="I35" s="9">
-        <v>42220</v>
+        <v>42229</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="13"/>
       <c r="D36" s="13"/>
       <c r="E36" s="13"/>
-      <c r="F36" s="12"/>
+      <c r="F36" s="17"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
@@ -1493,7 +1500,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B37" s="3">
         <v>3</v>
@@ -1502,22 +1509,22 @@
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="3" t="s">
-        <v>44</v>
+      <c r="G37" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="H37" s="9">
-        <v>42220</v>
+        <v>42229</v>
       </c>
       <c r="I37" s="9">
-        <v>42220</v>
+        <v>42230</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B38" s="3">
         <v>6</v>
@@ -1533,15 +1540,17 @@
         <v>10</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H38" s="9">
-        <v>42221</v>
+        <v>42226</v>
       </c>
       <c r="I38" s="9">
-        <v>42223</v>
-      </c>
-      <c r="J38" s="3"/>
+        <v>42227</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
@@ -1557,7 +1566,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="11">
@@ -1579,7 +1588,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B41" s="3">
         <v>3</v>
@@ -1589,7 +1598,7 @@
       <c r="E41" s="13"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H41" s="9">
         <v>42219</v>
@@ -1598,7 +1607,7 @@
         <v>42219</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -1615,7 +1624,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B43" s="3">
         <v>1</v>
@@ -1625,7 +1634,7 @@
       <c r="E43" s="13"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H43" s="9">
         <v>42219</v>
@@ -1634,12 +1643,12 @@
         <v>42219</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="13"/>
@@ -1653,7 +1662,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B45" s="3">
         <v>4</v>
@@ -1663,7 +1672,7 @@
       <c r="E45" s="13"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H45" s="9">
         <v>42219</v>
@@ -1672,12 +1681,12 @@
         <v>42219</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B46" s="3">
         <v>1</v>
@@ -1687,7 +1696,7 @@
       <c r="E46" s="13"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H46" s="9">
         <v>42220</v>
@@ -1696,12 +1705,12 @@
         <v>42220</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="13"/>
@@ -1715,7 +1724,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B48" s="3">
         <v>3</v>
@@ -1725,7 +1734,7 @@
       <c r="E48" s="13"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H48" s="9">
         <v>42220</v>
@@ -1734,12 +1743,12 @@
         <v>42220</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B49" s="3">
         <v>1</v>
@@ -1749,7 +1758,7 @@
       <c r="E49" s="13"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H49" s="9">
         <v>42220</v>
@@ -1758,12 +1767,12 @@
         <v>42220</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="13"/>
@@ -1777,7 +1786,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B51" s="3">
         <v>3</v>
@@ -1787,7 +1796,7 @@
       <c r="E51" s="13"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H51" s="9">
         <v>42220</v>
@@ -1796,12 +1805,12 @@
         <v>42220</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B52" s="3">
         <v>3</v>
@@ -1811,7 +1820,7 @@
       <c r="E52" s="13"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H52" s="9">
         <v>42221</v>
@@ -1820,12 +1829,12 @@
         <v>42222</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B53" s="3">
         <v>4</v>
@@ -1835,7 +1844,7 @@
       <c r="E53" s="12"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H53" s="9">
         <v>42221</v>
@@ -1844,7 +1853,7 @@
         <v>42223</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
@@ -1861,7 +1870,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -1877,7 +1886,7 @@
     </row>
     <row r="56" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B56" s="3">
         <v>3</v>
@@ -1889,7 +1898,7 @@
         <v>3</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H56" s="9">
         <v>42221</v>
@@ -1898,12 +1907,12 @@
         <v>42221</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B57" s="3">
         <v>5</v>
@@ -1915,33 +1924,107 @@
         <v>5</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H57" s="9">
         <v>42221</v>
       </c>
       <c r="I57" s="9">
-        <v>42221</v>
+        <v>42223</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="A58" s="2"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
-      <c r="F58" s="7">
-        <v>158</v>
-      </c>
+      <c r="F58" s="3"/>
       <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
-      <c r="I58" s="3"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="9"/>
       <c r="J58" s="3"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="9"/>
+      <c r="I59" s="9"/>
+      <c r="J59" s="3"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B60" s="3">
+        <v>10</v>
+      </c>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3">
+        <v>10</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H60" s="9">
+        <v>42228</v>
+      </c>
+      <c r="I60" s="9">
+        <v>42229</v>
+      </c>
+      <c r="J60" s="3"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B61" s="3">
+        <v>10</v>
+      </c>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3">
+        <v>10</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H61" s="9">
+        <v>42229</v>
+      </c>
+      <c r="I61" s="9">
+        <v>42230</v>
+      </c>
+      <c r="J61" s="3"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="7">
+        <v>178</v>
+      </c>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="17">
@@ -1952,10 +2035,10 @@
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="E16:E18"/>
     <mergeCell ref="C19:C24"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="C40:C53"/>
     <mergeCell ref="D40:D53"/>

</xml_diff>